<commit_message>
fix import student via excel files
</commit_message>
<xml_diff>
--- a/cypress/fixtures/students_import/correct_students_template.xlsx
+++ b/cypress/fixtures/students_import/correct_students_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NOMENA\HEI\HEI-ADMIN\hei-admin\hei-admin-test\cypress\fixtures\students_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A2F706-61E2-407D-9564-6CC77D7674C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BEE670-C2E9-4975-AF8A-EC6B2DAE8CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>ref</t>
   </si>
@@ -69,37 +69,13 @@
     <t>Jeanne</t>
   </si>
   <si>
-    <t>Jean</t>
+    <t>STD000130-PROJ1-G18</t>
   </si>
   <si>
-    <t>Pierre</t>
+    <t>STD000131-PROJ1-G18</t>
   </si>
   <si>
-    <t>Hélène</t>
-  </si>
-  <si>
-    <t>Patrice</t>
-  </si>
-  <si>
-    <t>STD000560-PROJ1-G18</t>
-  </si>
-  <si>
-    <t>STD000561-PROJ1-G18</t>
-  </si>
-  <si>
-    <t>STD000562-PROJ1-G18</t>
-  </si>
-  <si>
-    <t>STD000563-PROJ1-G18</t>
-  </si>
-  <si>
-    <t>STD000564-PROJ1-G18</t>
-  </si>
-  <si>
-    <t>STD000565-PROJ1-G18</t>
-  </si>
-  <si>
-    <t>STD000566-PROJ1-G18</t>
+    <t>STD000132-PROJ1-G18</t>
   </si>
 </sst>
 </file>
@@ -353,7 +329,7 @@
   <dimension ref="A1:G999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -389,7 +365,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -398,8 +374,8 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="str">
-        <f t="shared" ref="D2:D8" si="0">CONCATENATE("user",A2,"@hei.school")</f>
-        <v>userSTD000560-PROJ1-G18@hei.school</v>
+        <f>CONCATENATE("user",A2,"@hei.school")</f>
+        <v>userSTD000130-PROJ1-G18@hei.school</v>
       </c>
       <c r="E2" s="5">
         <v>44621</v>
@@ -411,7 +387,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -420,8 +396,8 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>userSTD000561-PROJ1-G18@hei.school</v>
+        <f t="shared" ref="D2:D8" si="0">CONCATENATE("user",A3,"@hei.school")</f>
+        <v>userSTD000131-PROJ1-G18@hei.school</v>
       </c>
       <c r="E3" s="5">
         <v>44622</v>
@@ -433,7 +409,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -443,7 +419,7 @@
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>userSTD000562-PROJ1-G18@hei.school</v>
+        <v>userSTD000132-PROJ1-G18@hei.school</v>
       </c>
       <c r="E4" s="5">
         <v>44623</v>
@@ -454,91 +430,39 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>userSTD000563-PROJ1-G18@hei.school</v>
-      </c>
-      <c r="E5" s="5">
-        <v>44624</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>userSTD000564-PROJ1-G18@hei.school</v>
-      </c>
-      <c r="E6" s="5">
-        <v>44625</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>userSTD000565-PROJ1-G18@hei.school</v>
-      </c>
-      <c r="E7" s="5">
-        <v>44626</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>userSTD000566-PROJ1-G18@hei.school</v>
-      </c>
-      <c r="E8" s="5">
-        <v>44627</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="3"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>